<commit_message>
login and model changes
</commit_message>
<xml_diff>
--- a/python/sample_data.xlsx
+++ b/python/sample_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Major Project\Major_project\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BE86D6-9F16-43AB-84E3-33ABC665F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85957850-D5BD-4BA9-9F78-F6FBFC4E8BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F38F0ED0-BAAF-4224-9CC6-4493E6D53C11}"/>
   </bookViews>
@@ -769,7 +769,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -780,6 +812,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0315B99C-6D47-43ED-809A-DFD01965FCFE}" name="Table1" displayName="Table1" ref="A1:F1757" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F1757" xr:uid="{0315B99C-6D47-43ED-809A-DFD01965FCFE}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8B21945F-0B2A-482F-9A47-AFEE3FEB0AFC}" name="state" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1CC60C4A-7016-418B-B944-E5E29D664910}" name="category" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{05BA585B-9753-4271-B4AA-B14BE4931BA6}" name="rating" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FBAD3143-4F4B-4D60-BBE5-D4F5D35E4CCF}" name="place1" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E3A8641D-EB6D-4ABC-BEEC-CBD15AC95EC2}" name="place2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{57B02575-5EF1-49FC-9562-0A8B52B12A86}" name="place3" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1081,15 +1128,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC30233F-FD10-45B0-B98D-DF00BE02BF23}">
   <dimension ref="A1:F1757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1308" workbookViewId="0">
-      <selection activeCell="D1314" sqref="D1314"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -36235,5 +36283,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>